<commit_message>
feat: Add direction handling for divergences in cruzar function
</commit_message>
<xml_diff>
--- a/output/cruzamento.xlsx
+++ b/output/cruzamento.xlsx
@@ -542,7 +542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="9" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -577,6 +578,11 @@
           <t>dif_rel</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>dir</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -594,6 +600,11 @@
       </c>
       <c r="D2" s="3" t="n">
         <v>5.517698016398227e-05</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>MENOR</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Enhance orcamento loading to handle duplicate entries and update cruzar function for consistent key usage
</commit_message>
<xml_diff>
--- a/output/cruzamento.xlsx
+++ b/output/cruzamento.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="1" max="1"/>
     <col width="9" customWidth="1" min="2" max="2"/>
-    <col width="46" customWidth="1" min="3" max="3"/>
+    <col width="80" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
-    <col width="46" customWidth="1" min="5" max="5"/>
+    <col width="80" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
     <col width="7" customWidth="1" min="7" max="7"/>
     <col width="9" customWidth="1" min="8" max="8"/>
-    <col width="23" customWidth="1" min="9" max="9"/>
+    <col width="9" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -497,38 +497,556 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01.12.01</t>
+          <t>97064</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SUDECAP</t>
+          <t>SINAPI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>VISTORIA CAUTELAR - ÁREA CONSTRUÍDA &lt;= 100M2</t>
+          <t>MONTAGEM E DESMONTAGEM DE ANDAIME TUBULAR TIPO "TORRE" (EXCLUSIVE ANDAIME E LIMPEZA). AF_03/2024</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>362.45</v>
+        <v>30.78</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>VISTORIA CAUTELAR - ÁREA CONSTRUÍDA &lt;= 100M2</t>
+          <t>MONTAGEM E DESMONTAGEM DE ANDAIME TUBULAR TIPO "TORRE" (EXCLUSIVE ANDAIME E LIMPEZA). AF_03/2024</t>
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>362.47</v>
+        <v>30.78</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>5.517698016398227e-05</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>100251</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Teste TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>88278</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MONTADOR DE ESTRUTURA METÁLICA COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>29.66</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>MONTADOR DE ESTRUTURA METÁLICA COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>29.66</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>88316</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SERVENTE COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>26.65</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>SERVENTE COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>26.65</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>88264</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ELETRICISTA COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>34.41</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ELETRICISTA COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>34.41</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>95332</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA ELETRICISTA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA ELETRICISTA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>95332</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA ELETRICISTA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA ELETRICISTA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>95344</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA MONTADOR DE ESTRUTURA METÁLICA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA MONTADOR DE ESTRUTURA METÁLICA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>95378</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA SERVENTE (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA SERVENTE (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>88278</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>MONTADOR DE ESTRUTURA METÁLICA COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>29.66</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>MONTADOR DE ESTRUTURA METÁLICA COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>29.66</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>95344</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA MONTADOR DE ESTRUTURA METÁLICA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA MONTADOR DE ESTRUTURA METÁLICA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>88316</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SERVENTE COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>26.65</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>SERVENTE COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>26.65</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>95378</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA SERVENTE (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>CURSO DE CAPACITAÇÃO PARA SERVENTE (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>100251</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>88316</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SINAPI</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SERVENTE COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>26.65</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>SERVENTE COM ENCARGOS COMPLEMENTARES</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>26.65</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -550,11 +1068,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="26" customWidth="1" min="2" max="2"/>
     <col width="9" customWidth="1" min="3" max="3"/>
-    <col width="23" customWidth="1" min="4" max="4"/>
-    <col width="7" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="5" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -587,25 +1105,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01.12.01</t>
+          <t>100251</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['VALOR_DIVERGENTE']</t>
+          <t>['DESCRICAO_DIVERGENTE']</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>5.517698016398227e-05</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>MENOR</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>